<commit_message>
add & update list
</commit_message>
<xml_diff>
--- a/response/Form Pengumpulan Tugas Sintech (Jawaban).xlsx
+++ b/response/Form Pengumpulan Tugas Sintech (Jawaban).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Timestamp</t>
   </si>
@@ -74,6 +74,27 @@
   </si>
   <si>
     <t>https://drive.google.com/open?id=1_GciE_cYMaffFJeWbHvHJRU5U3V9FdMw</t>
+  </si>
+  <si>
+    <t>dvndevin05@gmail.com</t>
+  </si>
+  <si>
+    <t>Athaya Devin Argyadama</t>
+  </si>
+  <si>
+    <t>X-IPA 1</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1Y3C1IELh8uIDZDZGV5vyLed_quhIV1bI</t>
+  </si>
+  <si>
+    <t>alfyanfakhrudi@gmail.com</t>
+  </si>
+  <si>
+    <t>Alfyan Cana Dwi Fakhrudi</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1l77MP4jDSCYw1bfzMKGJleJ99AoSJ1VC</t>
   </si>
 </sst>
 </file>
@@ -433,13 +454,49 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>44386.350098888885</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>44387.62598138889</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="E2"/>
     <hyperlink r:id="rId2" ref="E3"/>
     <hyperlink r:id="rId3" ref="E4"/>
     <hyperlink r:id="rId4" ref="E5"/>
+    <hyperlink r:id="rId5" ref="E6"/>
+    <hyperlink r:id="rId6" ref="E7"/>
   </hyperlinks>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>